<commit_message>
Add Student - Constructing the HTML Form
</commit_message>
<xml_diff>
--- a/me_docs/11.Add-Student.xlsx
+++ b/me_docs/11.Add-Student.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\JSP-Servlets-JDBC\me_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E698D44-50B4-48A9-AC92-7BABE9776CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459FFCA6-6CF0-44BE-A665-4212A99FB2B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="picture" sheetId="1" r:id="rId1"/>
-    <sheet name="Add Student Button" sheetId="2" r:id="rId2"/>
+    <sheet name="Setting up the Button" sheetId="2" r:id="rId2"/>
+    <sheet name="Constructing the HTML Form" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Add Student</t>
   </si>
@@ -37,7 +38,19 @@
     <t>Add add-student-form.jsp file</t>
   </si>
   <si>
-    <t>Check click Add Button</t>
+    <t>stylesheet</t>
+  </si>
+  <si>
+    <t>Coppy add-student-style.css to project</t>
+  </si>
+  <si>
+    <t>body</t>
+  </si>
+  <si>
+    <t>Check by access URL http://localhost:8080/web-student-tracker/add-student-form.jsp</t>
+  </si>
+  <si>
+    <t>Check click Add Button and check redirect to add-student-form.jsp</t>
   </si>
 </sst>
 </file>
@@ -443,6 +456,231 @@
         <a:xfrm>
           <a:off x="609600" y="30861000"/>
           <a:ext cx="4923809" cy="1295238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>141790</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>8929</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4752516D-1F61-490E-992C-7B4483B357CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="8676190" cy="4771429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>113905</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>113667</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8990BD8D-9E8D-453D-8013-19E9A76AA4C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="5524500"/>
+          <a:ext cx="3161905" cy="5066667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>284569</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>18211</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95070777-9961-4EF3-B0F4-72D046024791}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="590550" y="11020425"/>
+          <a:ext cx="9447619" cy="6714286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>217905</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>113762</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DADAA89-247A-422D-B712-996EB39D390C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="18097500"/>
+          <a:ext cx="9361905" cy="4304762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>313143</xdr:colOff>
+      <xdr:row>137</xdr:row>
+      <xdr:rowOff>75762</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B76B174-5D48-477D-BE09-B6018D68EF84}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="22669500"/>
+          <a:ext cx="9457143" cy="3504762"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -734,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C62E0D5-5BEC-478C-84E8-5C1367B3DD38}">
   <dimension ref="A2:A143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="B171" sqref="B171"/>
+    <sheetView topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="A144" sqref="A144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,7 +995,43 @@
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B49D6C0-9790-4B0C-8696-E26949224141}">
+  <dimension ref="A2:A95"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="E144" sqref="E144"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Student - Developing the Servlet
</commit_message>
<xml_diff>
--- a/me_docs/11.Add-Student.xlsx
+++ b/me_docs/11.Add-Student.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\JSP-Servlets-JDBC\me_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459FFCA6-6CF0-44BE-A665-4212A99FB2B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88137C9-819B-4E84-8983-8DB2C62E76CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="picture" sheetId="1" r:id="rId1"/>
     <sheet name="Setting up the Button" sheetId="2" r:id="rId2"/>
     <sheet name="Constructing the HTML Form" sheetId="3" r:id="rId3"/>
+    <sheet name="Developing the Servlet" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Add Student</t>
   </si>
@@ -51,6 +52,30 @@
   </si>
   <si>
     <t>Check click Add Button and check redirect to add-student-form.jsp</t>
+  </si>
+  <si>
+    <t>config add Url in list-students.jsp</t>
+  </si>
+  <si>
+    <t>Create Create AddStudentControllerServlet</t>
+  </si>
+  <si>
+    <t>Restart Server</t>
+  </si>
+  <si>
+    <t>Access URL to test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">redirected to add page </t>
+  </si>
+  <si>
+    <t>doPost method</t>
+  </si>
+  <si>
+    <t>init</t>
+  </si>
+  <si>
+    <t>addStudent is created</t>
   </si>
 </sst>
 </file>
@@ -160,6 +185,270 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>179809</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>9071</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{857AEFBD-BEA8-487F-8656-78045BEC8408}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="6667500"/>
+          <a:ext cx="9323809" cy="3628571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>246781</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>27929</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50602C5A-47D5-4023-93DF-B620E7423264}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="10858500"/>
+          <a:ext cx="6952381" cy="5171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>589943</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>180262</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E81C5F84-B3E2-45B2-8506-6F9C655CA834}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="16192500"/>
+          <a:ext cx="4857143" cy="5704762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>475581</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>189905</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B38B943-63FE-4211-929F-43ACDD666542}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="22098000"/>
+          <a:ext cx="5352381" cy="4761905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>143</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>160762</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>190071</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3BF7CD8-4FAB-4A35-B454-44D54934C100}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="27241500"/>
+          <a:ext cx="9304762" cy="3428571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>162</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>47009</xdr:colOff>
+      <xdr:row>168</xdr:row>
+      <xdr:rowOff>152238</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D517468B-C153-4497-8099-EBD31768641C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="30861000"/>
+          <a:ext cx="4923809" cy="1295238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -171,19 +460,19 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D9AA847-4DA6-4E79-BD64-D1BE50A55239}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA26C699-9099-428F-9B67-4B5AEAAA42A4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -192,270 +481,6 @@
         <a:xfrm>
           <a:off x="609600" y="381000"/>
           <a:ext cx="9733333" cy="5857143"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>179809</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>9071</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{857AEFBD-BEA8-487F-8656-78045BEC8408}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="609600" y="6667500"/>
-          <a:ext cx="9323809" cy="3628571"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>246781</xdr:colOff>
-      <xdr:row>84</xdr:row>
-      <xdr:rowOff>27929</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50602C5A-47D5-4023-93DF-B620E7423264}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="609600" y="10858500"/>
-          <a:ext cx="6952381" cy="5171429"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>589943</xdr:colOff>
-      <xdr:row>114</xdr:row>
-      <xdr:rowOff>180262</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E81C5F84-B3E2-45B2-8506-6F9C655CA834}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="609600" y="16192500"/>
-          <a:ext cx="4857143" cy="5704762"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>116</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>475581</xdr:colOff>
-      <xdr:row>140</xdr:row>
-      <xdr:rowOff>189905</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B38B943-63FE-4211-929F-43ACDD666542}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="609600" y="22098000"/>
-          <a:ext cx="5352381" cy="4761905"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>143</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>160762</xdr:colOff>
-      <xdr:row>160</xdr:row>
-      <xdr:rowOff>190071</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3BF7CD8-4FAB-4A35-B454-44D54934C100}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="609600" y="27241500"/>
-          <a:ext cx="9304762" cy="3428571"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>162</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>47009</xdr:colOff>
-      <xdr:row>168</xdr:row>
-      <xdr:rowOff>152238</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D517468B-C153-4497-8099-EBD31768641C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="609600" y="30861000"/>
-          <a:ext cx="4923809" cy="1295238"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -559,50 +584,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>284569</xdr:colOff>
-      <xdr:row>93</xdr:row>
-      <xdr:rowOff>18211</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95070777-9961-4EF3-B0F4-72D046024791}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="590550" y="11020425"/>
-          <a:ext cx="9447619" cy="6714286"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>95</xdr:row>
@@ -628,7 +609,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -672,7 +653,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -681,6 +662,627 @@
         <a:xfrm>
           <a:off x="609600" y="22669500"/>
           <a:ext cx="9457143" cy="3504762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>275048</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>18214</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{226BF6DB-3BA7-4105-9A28-E71D1D7324D1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="11049000"/>
+          <a:ext cx="9419048" cy="6685714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>589409</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>75357</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA92ABD3-6EE5-47BA-AAB8-63FF49A6C120}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="9123809" cy="6742857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>246781</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>151738</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{415972E6-D8BE-48B1-9CA0-81C16AD0F215}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="7620000"/>
+          <a:ext cx="6952381" cy="5295238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>8914</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>171000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{562FF228-D0EC-4E0C-8AA3-56F542F2D6DA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="13144500"/>
+          <a:ext cx="4885714" cy="3600000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>27962</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>75619</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BF66B89-B9F6-4C81-A930-9DDC5993451C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="16954500"/>
+          <a:ext cx="4904762" cy="4647619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>8914</xdr:colOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>75619</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F42CC83-8E4F-47E7-924F-ABE32BD8219C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="21907500"/>
+          <a:ext cx="4885714" cy="4647619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>141409</xdr:colOff>
+      <xdr:row>167</xdr:row>
+      <xdr:rowOff>18405</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F3A17FA-E4E7-4AEC-9408-44C4BB105FF1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="26670000"/>
+          <a:ext cx="11723809" cy="5161905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>169</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>246171</xdr:colOff>
+      <xdr:row>200</xdr:row>
+      <xdr:rowOff>27833</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C6075CE-A2D3-47CD-B442-E97C4D7615B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="32194500"/>
+          <a:ext cx="11828571" cy="5933333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>203</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>284267</xdr:colOff>
+      <xdr:row>229</xdr:row>
+      <xdr:rowOff>170809</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E75FA69-C9C9-4B33-AE03-38146CB20C8F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="38671500"/>
+          <a:ext cx="11866667" cy="5123809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>232</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>179809</xdr:colOff>
+      <xdr:row>250</xdr:row>
+      <xdr:rowOff>171000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72598BEB-7D93-4B4C-AEAA-70B9A70C8C3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="44196000"/>
+          <a:ext cx="9323809" cy="3600000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>253</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>198857</xdr:colOff>
+      <xdr:row>273</xdr:row>
+      <xdr:rowOff>190000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FABBABA-B948-4EA3-B6B2-F7F266E0C344}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="48196500"/>
+          <a:ext cx="9342857" cy="4000000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>276</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>170286</xdr:colOff>
+      <xdr:row>303</xdr:row>
+      <xdr:rowOff>85071</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D05927C2-8ED1-4574-A699-2BE7DEBA6AC1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="52578000"/>
+          <a:ext cx="9314286" cy="5228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>306</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>93790</xdr:colOff>
+      <xdr:row>333</xdr:row>
+      <xdr:rowOff>104119</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D0775D8-8940-4FD1-8D8C-D3C1E56C8B3D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="58293000"/>
+          <a:ext cx="11676190" cy="5247619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>336</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>84419</xdr:colOff>
+      <xdr:row>363</xdr:row>
+      <xdr:rowOff>123167</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E30E5B96-F1CE-4E9A-8247-6C2E021FE6AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="64008000"/>
+          <a:ext cx="10447619" cy="5266667"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -972,8 +1574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C62E0D5-5BEC-478C-84E8-5C1367B3DD38}">
   <dimension ref="A2:A143"/>
   <sheetViews>
-    <sheetView topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="A144" sqref="A144"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,8 +1610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B49D6C0-9790-4B0C-8696-E26949224141}">
   <dimension ref="A2:A95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="E144" sqref="E144"/>
+    <sheetView topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,4 +1640,60 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F550C8A9-E691-4A95-A0AA-492B3F217C95}">
+  <dimension ref="A2:B336"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A355" workbookViewId="0">
+      <selection activeCell="B366" sqref="B366"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="253" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B253" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Student - Creating the JDBC Code
</commit_message>
<xml_diff>
--- a/me_docs/11.Add-Student.xlsx
+++ b/me_docs/11.Add-Student.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\JSP-Servlets-JDBC\me_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88137C9-819B-4E84-8983-8DB2C62E76CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A605CAA-FE41-468B-9480-3A2496E96591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="picture" sheetId="1" r:id="rId1"/>
     <sheet name="Setting up the Button" sheetId="2" r:id="rId2"/>
     <sheet name="Constructing the HTML Form" sheetId="3" r:id="rId3"/>
     <sheet name="Developing the Servlet" sheetId="4" r:id="rId4"/>
+    <sheet name="Creating the JDBC Code" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Add Student</t>
   </si>
@@ -76,6 +77,27 @@
   </si>
   <si>
     <t>addStudent is created</t>
+  </si>
+  <si>
+    <t>Go to addStudent method to code</t>
+  </si>
+  <si>
+    <t>addStudent method</t>
+  </si>
+  <si>
+    <t>listStudents method</t>
+  </si>
+  <si>
+    <t>Reset Server</t>
+  </si>
+  <si>
+    <t>Access url to test</t>
+  </si>
+  <si>
+    <t>Access url to test redirect to list page after save</t>
+  </si>
+  <si>
+    <t>Check database data saved</t>
   </si>
 </sst>
 </file>
@@ -1283,6 +1305,583 @@
         <a:xfrm>
           <a:off x="609600" y="64008000"/>
           <a:ext cx="10447619" cy="5266667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>366</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>227124</xdr:colOff>
+      <xdr:row>393</xdr:row>
+      <xdr:rowOff>37452</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2B161AF-96DC-44E4-AAD1-E2173A98FEE3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="69723000"/>
+          <a:ext cx="11809524" cy="5180952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>394</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>112838</xdr:colOff>
+      <xdr:row>421</xdr:row>
+      <xdr:rowOff>56500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{488C3C51-2D1D-47CB-83BF-9C658D1E9BD5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="75057000"/>
+          <a:ext cx="11695238" cy="5200000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>423</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>74743</xdr:colOff>
+      <xdr:row>450</xdr:row>
+      <xdr:rowOff>8881</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AFE3A87-B6C6-4E8E-A1FB-09223D47E150}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="80581500"/>
+          <a:ext cx="11657143" cy="5152381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>451</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>284419</xdr:colOff>
+      <xdr:row>478</xdr:row>
+      <xdr:rowOff>123167</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A1D8FC4-44C9-4F28-A0DA-B7C55AAD798C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="85915500"/>
+          <a:ext cx="10647619" cy="5266667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>481</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>256228</xdr:colOff>
+      <xdr:row>508</xdr:row>
+      <xdr:rowOff>46976</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0AFAA3E-D7E4-43CF-B862-76972AB68505}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="91630500"/>
+          <a:ext cx="7571428" cy="5190476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>511</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>170286</xdr:colOff>
+      <xdr:row>532</xdr:row>
+      <xdr:rowOff>18548</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77CCCFB8-CA85-4E00-8040-8589E9CD9BED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="97345500"/>
+          <a:ext cx="9314286" cy="4019048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>533</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>160762</xdr:colOff>
+      <xdr:row>551</xdr:row>
+      <xdr:rowOff>66238</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47350786-82FF-45BF-9904-FCF981361DD2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="101536500"/>
+          <a:ext cx="9304762" cy="3495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>55695</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>8881</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E6FB1CF-B08E-4C73-AA2F-5A48D12C14B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="11638095" cy="5152381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>455771</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>189857</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C75AFBA6-73C0-43D6-85D6-F18EF456A545}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="5905500"/>
+          <a:ext cx="11428571" cy="5142857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>125414</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D475ED9-645E-4D2F-AC0B-89426C55150A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="11239500"/>
+          <a:ext cx="11258550" cy="4506914"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>170286</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>132857</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35CC8BAF-D045-43FE-B03E-E1F16BA2F3A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="16192500"/>
+          <a:ext cx="9314286" cy="3942857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>189333</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>37643</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58640756-4161-4F00-896A-9BF63E3CBED8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="20383500"/>
+          <a:ext cx="9333333" cy="3657143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>227809</xdr:colOff>
+      <xdr:row>147</xdr:row>
+      <xdr:rowOff>18619</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{788619A7-BDFF-4BD5-95F7-B1ABBA22BD39}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="24574500"/>
+          <a:ext cx="6323809" cy="3447619"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1644,10 +2243,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F550C8A9-E691-4A95-A0AA-492B3F217C95}">
-  <dimension ref="A2:B336"/>
+  <dimension ref="A2:B511"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A355" workbookViewId="0">
-      <selection activeCell="B366" sqref="B366"/>
+    <sheetView topLeftCell="A541" workbookViewId="0">
+      <selection activeCell="A512" sqref="A512"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1692,6 +2291,57 @@
         <v>15</v>
       </c>
     </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A366" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A481" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="511" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A511" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F55FBAF5-90EA-4127-9167-578BDDC7FAB1}">
+  <dimension ref="A2:A129"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="D151" sqref="D151"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>